<commit_message>
update method for update validate input reset password.
</commit_message>
<xml_diff>
--- a/testData/resetPasswordUserData - Copy.xlsx
+++ b/testData/resetPasswordUserData - Copy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srajendran\git\seleniumJavaRepo\InsuranceNow_v1.0\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srajendran\iNow_Reusalble\InsuranceNowReusable\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE08CE63-CD61-4F3F-B904-4C756973473D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FEF13F-C2D7-4E2A-A0D5-30A9BF8EBB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{838B1716-2769-449B-83C2-A98D2BE273E4}"/>
+    <workbookView xWindow="-30828" yWindow="-1320" windowWidth="30936" windowHeight="16776" xr2:uid="{838B1716-2769-449B-83C2-A98D2BE273E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1332,8 +1332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4C1CEF3-1EB1-498B-ABFA-BD26A2AA477F}">
   <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>